<commit_message>
Changing nodes to 8
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -10,54 +10,70 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$55</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$56:$B$65</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$73</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$74:$C$83</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$91</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$92:$B$101</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$91</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$92:$C$101</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$181</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$182:$B$191</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$C$181</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$C$182:$C$191</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$55</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$109</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$110:$B$119</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$109</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$110:$C$119</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$127</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$128:$B$137</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$127</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$C$128:$C$137</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$B$145</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$146:$B$155</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$56:$C$65</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$C$145</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$146:$C$155</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$B$163</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$B$164:$B$173</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$C$163</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$C$164:$C$173</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$B$19:$B$28</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$C$18</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$C$19:$C$28</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$B$37</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$B$38:$B$47</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$C$37</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$C$38:$C$47</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$B$199</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$B$200:$B$209</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$C$199</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$C$200:$C$209</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$73</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$74:$B$83</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$253</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$254:$B$263</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$37</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$38:$C$47</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$217</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$218:$B$227</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$217</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$218:$C$227</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$55</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$56:$B$65</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$C$55</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$C$56:$C$65</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$253</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$73</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$B$74:$B$83</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$73</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$74:$C$83</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$91</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$92:$B$101</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$91</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$C$92:$C$101</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$2:$B$11</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$254:$C$263</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$2:$C$11</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$B$145</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$B$146:$B$155</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$C$145</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$C$146:$C$155</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$B$109</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$B$110:$B$119</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$C$109</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$C$110:$C$119</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$B$127</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$B$128:$B$137</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$C$127</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$C$128:$C$137</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$B$163</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$B$164:$B$173</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$C$163</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$C$164:$C$173</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$B$181</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$B$182:$B$191</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$19:$B$28</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$C$181</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$C$182:$C$191</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$B$199</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$B$200:$B$209</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$C$199</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$C$200:$C$209</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$B$271</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$B$272:$B$281</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$C$271</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$C$272:$C$281</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$18</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$B$235</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$B$236:$B$245</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$C$235</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$C$236:$C$245</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$19:$C$28</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$37</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$38:$B$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -69,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="63">
   <si>
     <t>Default</t>
   </si>
@@ -240,6 +256,24 @@
   </si>
   <si>
     <t>Gaussian distribution</t>
+  </si>
+  <si>
+    <t>Note: Mutating change is using Gaussian distribution with mean = 0.4 and</t>
+  </si>
+  <si>
+    <t>Experiment No 12</t>
+  </si>
+  <si>
+    <t>Mutation rate</t>
+  </si>
+  <si>
+    <t>Experiment No 13</t>
+  </si>
+  <si>
+    <t>Experiment No 14</t>
+  </si>
+  <si>
+    <t>Experiment No 15</t>
   </si>
 </sst>
 </file>
@@ -500,331 +534,6 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.37</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{74230CD1-8691-40FC-9C3B-AF93DCBFFA84}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.36</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{7D898464-E2A7-4570-A0F8-B571BD39D444}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx10.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.35</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.32</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.34</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx11.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx12.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.45</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.47</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.44</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.46</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.42</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
-              <cx:v>Fitness on training</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
-              <cx:v>Fitness on testing</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-    </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
         <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
@@ -881,7 +590,373 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx10.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.45</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.47</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.44</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.46</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx11.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.49</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.51</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.50</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx12.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.53</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.55</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.52</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.54</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx13.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx14.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.61</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.63</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.60</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.62</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx15.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx16.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.57</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.59</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.56</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.58</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
@@ -932,17 +1007,17 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -953,7 +1028,7 @@
         <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>Fitness on training</cx:v>
             </cx:txData>
           </cx:tx>
@@ -966,7 +1041,7 @@
         <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>Fitness on testing</cx:v>
             </cx:txData>
           </cx:tx>
@@ -983,7 +1058,68 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.29</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.31</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{74230CD1-8691-40FC-9C3B-AF93DCBFFA84}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{7D898464-E2A7-4570-A0F8-B571BD39D444}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
@@ -1034,7 +1170,7 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
@@ -1052,7 +1188,7 @@
     <cx:title pos="t" align="ctr" overlay="0"/>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}">
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.24</cx:f>
@@ -1065,7 +1201,7 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}">
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.26</cx:f>
@@ -1079,32 +1215,23 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0" hidden="1">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
     </cx:plotArea>
     <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.29</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.31</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1115,7 +1242,7 @@
         <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.28</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>Fitness on training</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1128,7 +1255,109 @@
         <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.41</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.43</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:v>Fitness on testing</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx9.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.33</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.35</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{EDB0B30E-52BA-427B-8789-731E002A604C}" formatIdx="0">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.32</cx:f>
+              <cx:v>Fitness on training</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" hidden="1" uniqueId="{E142BA58-EAD1-47FD-B199-F07609EA5D86}" formatIdx="1">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.34</cx:f>
               <cx:v>Fitness on testing</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1266,6 +1495,166 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3084,6 +3473,1950 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8275,6 +10608,278 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="17" name="Chart 16"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="18" name="Chart 17"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="19" name="Chart 18"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>270</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="20" name="Chart 19"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8541,10 +11146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="C207" sqref="C207"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200:XFD209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10364,7 +12969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="13" t="s">
         <v>3</v>
       </c>
@@ -10387,7 +12992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="14" t="s">
         <v>4</v>
       </c>
@@ -10410,7 +13015,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="14" t="s">
         <v>5</v>
       </c>
@@ -10433,7 +13038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="14" t="s">
         <v>6</v>
       </c>
@@ -10456,7 +13061,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="14" t="s">
         <v>7</v>
       </c>
@@ -10473,7 +13078,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="14" t="s">
         <v>11</v>
       </c>
@@ -10493,7 +13098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="14" t="s">
         <v>12</v>
       </c>
@@ -10507,7 +13112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="14" t="s">
         <v>9</v>
       </c>
@@ -10521,7 +13126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
         <v>10</v>
       </c>
@@ -10532,7 +13137,7 @@
         <v>5.0391399142971603E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="14" t="s">
         <v>13</v>
       </c>
@@ -11396,7 +14001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="13" t="s">
         <v>3</v>
       </c>
@@ -11419,7 +14024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
         <v>4</v>
       </c>
@@ -11442,7 +14047,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
         <v>5</v>
       </c>
@@ -11465,7 +14070,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="14" t="s">
         <v>6</v>
       </c>
@@ -11488,7 +14093,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="14" t="s">
         <v>7</v>
       </c>
@@ -11505,7 +14110,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="14" t="s">
         <v>11</v>
       </c>
@@ -11523,7 +14128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
         <v>12</v>
       </c>
@@ -11537,7 +14142,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="14" t="s">
         <v>9</v>
       </c>
@@ -11551,27 +14156,35 @@
         <v>41</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B208" s="6"/>
-      <c r="C208" s="7"/>
+      <c r="B208" s="6">
+        <v>1.1479557488997399E-2</v>
+      </c>
+      <c r="C208" s="7">
+        <v>3.1743583517208802E-2</v>
+      </c>
       <c r="I208" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B209" s="8"/>
-      <c r="C209" s="9"/>
+      <c r="B209" s="8">
+        <v>9.0386305694420896E-3</v>
+      </c>
+      <c r="C209" s="9">
+        <v>2.2822490131261999E-2</v>
+      </c>
       <c r="I209" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" s="15" t="s">
         <v>8</v>
       </c>
@@ -11581,20 +14194,1064 @@
       </c>
       <c r="C210" s="10">
         <f>MEDIAN(C200:C209)</f>
-        <v>2.17328186220467E-2</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.1922579329728901E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B211" s="3">
         <f>AVERAGE(B200:B209)</f>
-        <v>1.1224587238887418E-2</v>
+        <v>1.1031488596953885E-2</v>
       </c>
       <c r="C211" s="3">
         <f>AVERAGE(C200:C209)</f>
-        <v>2.9758216392938214E-2</v>
+        <v>2.9263180479197647E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A214" s="17"/>
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
+      <c r="D214" s="17"/>
+      <c r="E214" s="17"/>
+      <c r="F214" s="17"/>
+      <c r="G214" s="17"/>
+      <c r="H214" s="17"/>
+      <c r="I214" s="17"/>
+      <c r="J214" s="17"/>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A215" s="17"/>
+      <c r="B215" s="17"/>
+      <c r="C215" s="17"/>
+      <c r="D215" s="17"/>
+      <c r="E215" s="17"/>
+      <c r="F215" s="17"/>
+      <c r="G215" s="17"/>
+      <c r="H215" s="17"/>
+      <c r="I215" s="17"/>
+      <c r="J215" s="17"/>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A217" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B217" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C217" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F217" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I217" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218" s="4">
+        <v>1.23974169868748E-2</v>
+      </c>
+      <c r="C218" s="5">
+        <v>3.3995370007763898E-2</v>
+      </c>
+      <c r="E218" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F218" s="1">
+        <v>100</v>
+      </c>
+      <c r="H218" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I218" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B219" s="6">
+        <v>1.09968498097603E-2</v>
+      </c>
+      <c r="C219" s="7">
+        <v>1.52427999070262E-2</v>
+      </c>
+      <c r="E219" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F219" s="1">
+        <v>6</v>
+      </c>
+      <c r="H219" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I219" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B220" s="6">
+        <v>1.9256752164113801E-2</v>
+      </c>
+      <c r="C220" s="7">
+        <v>1.9201827523185801E-2</v>
+      </c>
+      <c r="E220" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F220" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H220" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I220" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B221" s="6">
+        <v>1.73897697737431E-2</v>
+      </c>
+      <c r="C221" s="7">
+        <v>1.9077708262042099E-2</v>
+      </c>
+      <c r="E221" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F221" s="1">
+        <v>1</v>
+      </c>
+      <c r="H221" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I221" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B222" s="6">
+        <v>2.2020408120500899E-2</v>
+      </c>
+      <c r="C222" s="7">
+        <v>5.99680787283942E-2</v>
+      </c>
+      <c r="E222" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F222" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B223" s="6">
+        <v>1.29578928675009E-2</v>
+      </c>
+      <c r="C223" s="7">
+        <v>3.4014529420338203E-2</v>
+      </c>
+      <c r="E223" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F223" s="1"/>
+      <c r="I223" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B224" s="6">
+        <v>1.73941095485401E-2</v>
+      </c>
+      <c r="C224" s="7">
+        <v>1.99317844408755E-2</v>
+      </c>
+      <c r="I224" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B225" s="6">
+        <v>4.2736956754312001E-2</v>
+      </c>
+      <c r="C225" s="7">
+        <v>8.9961735718014496E-2</v>
+      </c>
+      <c r="I225" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B226" s="6">
+        <v>1.30901323914997E-2</v>
+      </c>
+      <c r="C226" s="7">
+        <v>8.9618236706596605E-2</v>
+      </c>
+      <c r="I226" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B227" s="8">
+        <v>1.30572442955825E-2</v>
+      </c>
+      <c r="C227" s="9">
+        <v>2.40141245427123E-2</v>
+      </c>
+      <c r="I227" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A228" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B228" s="10">
+        <f>MEDIAN(B218:B227)</f>
+        <v>1.5239951082621401E-2</v>
+      </c>
+      <c r="C228" s="10">
+        <f>MEDIAN(C218:C227)</f>
+        <v>2.9004747275238101E-2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A229" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B229" s="3">
+        <f>AVERAGE(B218:B227)</f>
+        <v>1.8129753271242811E-2</v>
+      </c>
+      <c r="C229" s="3">
+        <f>AVERAGE(C218:C227)</f>
+        <v>4.0502619525694936E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A232" s="17"/>
+      <c r="B232" s="17"/>
+      <c r="C232" s="17"/>
+      <c r="D232" s="17"/>
+      <c r="E232" s="17"/>
+      <c r="F232" s="17"/>
+      <c r="G232" s="17"/>
+      <c r="H232" s="17"/>
+      <c r="I232" s="17"/>
+      <c r="J232" s="17"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A233" s="17"/>
+      <c r="B233" s="17"/>
+      <c r="C233" s="17"/>
+      <c r="D233" s="17"/>
+      <c r="E233" s="17"/>
+      <c r="F233" s="17"/>
+      <c r="G233" s="17"/>
+      <c r="H233" s="17"/>
+      <c r="I233" s="17"/>
+      <c r="J233" s="17"/>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A235" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B235" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C235" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F235" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I235" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236" s="4">
+        <v>3.9486508926472999E-2</v>
+      </c>
+      <c r="C236" s="5">
+        <v>0.11213827326482401</v>
+      </c>
+      <c r="E236" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F236" s="1">
+        <v>100</v>
+      </c>
+      <c r="H236" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I236" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237" s="6">
+        <v>2.7835812700541598E-2</v>
+      </c>
+      <c r="C237" s="7">
+        <v>8.9744330505027503E-2</v>
+      </c>
+      <c r="E237" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F237" s="1">
+        <v>6</v>
+      </c>
+      <c r="H237" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I237" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B238" s="6">
+        <v>1.41158469072858E-2</v>
+      </c>
+      <c r="C238" s="7">
+        <v>0.157551504939277</v>
+      </c>
+      <c r="E238" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F238" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H238" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I238" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B239" s="6">
+        <v>9.8970962193676206E-3</v>
+      </c>
+      <c r="C239" s="7">
+        <v>9.9093068672167807E-3</v>
+      </c>
+      <c r="E239" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F239" s="1">
+        <v>1</v>
+      </c>
+      <c r="H239" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I239" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B240" s="6">
+        <v>1.51920806299578E-2</v>
+      </c>
+      <c r="C240" s="7">
+        <v>1.8199688013822799E-2</v>
+      </c>
+      <c r="E240" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F240" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B241" s="6">
+        <v>2.9773395660575699E-2</v>
+      </c>
+      <c r="C241" s="7">
+        <v>4.1352824689795002E-2</v>
+      </c>
+      <c r="E241" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F241" s="1"/>
+      <c r="I241" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B242" s="6">
+        <v>1.2031981096196701E-2</v>
+      </c>
+      <c r="C242" s="7">
+        <v>1.83751562328579E-2</v>
+      </c>
+      <c r="I242" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B243" s="6">
+        <v>9.4136063681312908E-3</v>
+      </c>
+      <c r="C243" s="7">
+        <v>1.3860198029136701E-2</v>
+      </c>
+      <c r="I243" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B244" s="6">
+        <v>1.70317108661307E-2</v>
+      </c>
+      <c r="C244" s="7">
+        <v>2.17600571956547E-2</v>
+      </c>
+      <c r="I244" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B245" s="8">
+        <v>0.10531540173137099</v>
+      </c>
+      <c r="C245" s="9">
+        <v>0.20526260703144</v>
+      </c>
+      <c r="I245" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A246" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B246" s="10">
+        <f>MEDIAN(B236:B245)</f>
+        <v>1.6111895748044249E-2</v>
+      </c>
+      <c r="C246" s="10">
+        <f>MEDIAN(C236:C245)</f>
+        <v>3.1556440942724848E-2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A247" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B247" s="3">
+        <f>AVERAGE(B236:B245)</f>
+        <v>2.8009344110603119E-2</v>
+      </c>
+      <c r="C247" s="3">
+        <f>AVERAGE(C236:C245)</f>
+        <v>6.8815394676905256E-2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A250" s="17"/>
+      <c r="B250" s="17"/>
+      <c r="C250" s="17"/>
+      <c r="D250" s="17"/>
+      <c r="E250" s="17"/>
+      <c r="F250" s="17"/>
+      <c r="G250" s="17"/>
+      <c r="H250" s="17"/>
+      <c r="I250" s="17"/>
+      <c r="J250" s="17"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A251" s="17"/>
+      <c r="B251" s="17"/>
+      <c r="C251" s="17"/>
+      <c r="D251" s="17"/>
+      <c r="E251" s="17"/>
+      <c r="F251" s="17"/>
+      <c r="G251" s="17"/>
+      <c r="H251" s="17"/>
+      <c r="I251" s="17"/>
+      <c r="J251" s="17"/>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A253" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B253" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C253" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F253" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H253" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I253" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A254" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" s="4">
+        <v>4.4267325121839E-2</v>
+      </c>
+      <c r="C254" s="5">
+        <v>0.118234324019377</v>
+      </c>
+      <c r="E254" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F254" s="1">
+        <v>100</v>
+      </c>
+      <c r="H254" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I254" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A255" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B255" s="6">
+        <v>1.47702168820548E-2</v>
+      </c>
+      <c r="C255" s="7">
+        <v>1.4838787167348801E-2</v>
+      </c>
+      <c r="E255" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F255" s="1">
+        <v>6</v>
+      </c>
+      <c r="H255" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I255" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B256" s="6">
+        <v>1.15395606024638E-2</v>
+      </c>
+      <c r="C256" s="7">
+        <v>1.5097774235944401E-2</v>
+      </c>
+      <c r="E256" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F256" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H256" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I256" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B257" s="6">
+        <v>9.2694407932133408E-3</v>
+      </c>
+      <c r="C257" s="7">
+        <v>9.1405767061776295E-3</v>
+      </c>
+      <c r="E257" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F257" s="1">
+        <v>1</v>
+      </c>
+      <c r="H257" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I257" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B258" s="6">
+        <v>1.1635043297113699E-2</v>
+      </c>
+      <c r="C258" s="7">
+        <v>1.39751418979979E-2</v>
+      </c>
+      <c r="E258" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F258" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B259" s="6">
+        <v>1.22673597484434E-2</v>
+      </c>
+      <c r="C259" s="7">
+        <v>4.7698502857783501E-2</v>
+      </c>
+      <c r="E259" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F259" s="1"/>
+      <c r="I259" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B260" s="6">
+        <v>1.18205171985547E-2</v>
+      </c>
+      <c r="C260" s="7">
+        <v>1.20344102280507E-2</v>
+      </c>
+      <c r="I260" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B261" s="6">
+        <v>1.02995176351312E-2</v>
+      </c>
+      <c r="C261" s="7">
+        <v>3.9045353910019003E-2</v>
+      </c>
+      <c r="I261" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B262" s="6">
+        <v>9.9023297070014102E-3</v>
+      </c>
+      <c r="C262" s="7">
+        <v>2.1088511060517699E-2</v>
+      </c>
+      <c r="I262" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B263" s="8">
+        <v>1.00951615874008E-2</v>
+      </c>
+      <c r="C263" s="9">
+        <v>1.6860413583752301E-2</v>
+      </c>
+      <c r="I263" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A264" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B264" s="10">
+        <f>MEDIAN(B254:B263)</f>
+        <v>1.1587301949788749E-2</v>
+      </c>
+      <c r="C264" s="10">
+        <f>MEDIAN(C254:C263)</f>
+        <v>1.5979093909848349E-2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A265" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B265" s="3">
+        <f>AVERAGE(B254:B263)</f>
+        <v>1.4586647257321617E-2</v>
+      </c>
+      <c r="C265" s="3">
+        <f>AVERAGE(C254:C263)</f>
+        <v>3.0801379566696891E-2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A268" s="17"/>
+      <c r="B268" s="17"/>
+      <c r="C268" s="17"/>
+      <c r="D268" s="17"/>
+      <c r="E268" s="17"/>
+      <c r="F268" s="17"/>
+      <c r="G268" s="17"/>
+      <c r="H268" s="17"/>
+      <c r="I268" s="17"/>
+      <c r="J268" s="17"/>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A269" s="17"/>
+      <c r="B269" s="17"/>
+      <c r="C269" s="17"/>
+      <c r="D269" s="17"/>
+      <c r="E269" s="17"/>
+      <c r="F269" s="17"/>
+      <c r="G269" s="17"/>
+      <c r="H269" s="17"/>
+      <c r="I269" s="17"/>
+      <c r="J269" s="17"/>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A271" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B271" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C271" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H271" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I271" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A272" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B272" s="4">
+        <v>1.0511754816608701E-2</v>
+      </c>
+      <c r="C272" s="5">
+        <v>1.26079826366632E-2</v>
+      </c>
+      <c r="E272" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F272" s="1">
+        <v>100</v>
+      </c>
+      <c r="H272" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I272" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A273" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B273" s="6">
+        <v>1.17120206138061E-2</v>
+      </c>
+      <c r="C273" s="7">
+        <v>1.37566494363669E-2</v>
+      </c>
+      <c r="E273" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F273" s="1">
+        <v>8</v>
+      </c>
+      <c r="H273" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I273" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A274" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B274" s="6">
+        <v>8.1037624619801196E-3</v>
+      </c>
+      <c r="C274" s="7">
+        <v>1.38324876755592E-2</v>
+      </c>
+      <c r="E274" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F274" s="1">
+        <v>-1</v>
+      </c>
+      <c r="H274" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I274" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A275" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B275" s="6">
+        <v>1.64826550141907E-2</v>
+      </c>
+      <c r="C275" s="7">
+        <v>1.6723809957874598E-2</v>
+      </c>
+      <c r="E275" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F275" s="1">
+        <v>1</v>
+      </c>
+      <c r="H275" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I275" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A276" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B276" s="6">
+        <v>1.49283158861944E-2</v>
+      </c>
+      <c r="C276" s="7">
+        <v>2.11393408390235E-2</v>
+      </c>
+      <c r="E276" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F276" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A277" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B277" s="6">
+        <v>9.9590692242654596E-3</v>
+      </c>
+      <c r="C277" s="7">
+        <v>3.1762725902686799E-2</v>
+      </c>
+      <c r="E277" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F277" s="1"/>
+      <c r="I277" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A278" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B278" s="6">
+        <v>1.1865614714483001E-2</v>
+      </c>
+      <c r="C278" s="7">
+        <v>1.1705731090199199E-2</v>
+      </c>
+      <c r="I278" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A279" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B279" s="6">
+        <v>1.8620638514943499E-2</v>
+      </c>
+      <c r="C279" s="7">
+        <v>4.6001059895857802E-2</v>
+      </c>
+      <c r="I279" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A280" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B280" s="6">
+        <v>1.13704173894894E-2</v>
+      </c>
+      <c r="C280" s="7">
+        <v>1.39460659691262E-2</v>
+      </c>
+      <c r="I280" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A281" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B281" s="8">
+        <v>1.1340233141234999E-2</v>
+      </c>
+      <c r="C281" s="9">
+        <v>1.00447562533281E-2</v>
+      </c>
+      <c r="I281" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A282" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B282" s="10">
+        <f>MEDIAN(B272:B281)</f>
+        <v>1.154121900164775E-2</v>
+      </c>
+      <c r="C282" s="10">
+        <f>MEDIAN(C272:C281)</f>
+        <v>1.38892768223427E-2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A283" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B283" s="3">
+        <f>AVERAGE(B272:B281)</f>
+        <v>1.248944817771964E-2</v>
+      </c>
+      <c r="C283" s="3">
+        <f>AVERAGE(C272:C281)</f>
+        <v>1.9152060965668551E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>